<commit_message>
Prepared to commit as "new" maestro repo in GitHub maestrobpm organization
</commit_message>
<xml_diff>
--- a/scc-files/excel/person.xlsx
+++ b/scc-files/excel/person.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="581" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="581"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="person" sheetId="7" r:id="rId2"/>
-    <sheet name="res.usrs" sheetId="8" r:id="rId3"/>
+    <sheet name="res.users" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">person!$A$1:$H$25</definedName>
@@ -1851,39 +1851,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.25" style="66" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.19921875" style="66" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="40.8984375" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
         <v>203</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="AB1" s="29"/>
       <c r="AC1" s="30"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>209</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="69">
         <v>1</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="69">
         <v>1</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="69">
         <v>1</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="69">
         <v>1</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="69">
         <v>1</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="69">
         <v>1</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="69">
         <v>1</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A10" s="69">
         <v>1</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="69">
         <v>1</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="69">
         <v>1</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="69">
         <v>1</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="69">
         <v>1</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="69">
         <v>1</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="69">
         <v>1</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="69">
         <v>1</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="66" x14ac:dyDescent="0.25">
       <c r="A18" s="69">
         <v>1</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="69">
         <v>1</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="69">
         <v>1</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="69">
         <v>1</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="69">
         <v>1</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="69">
         <v>1</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70">
         <v>1</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>208</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B28" s="56"/>
       <c r="C28" s="1" t="s">
         <v>146</v>
@@ -4047,17 +4047,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.625" style="66" customWidth="1"/>
-    <col min="4" max="4" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.59765625" style="66" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>201</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
         <v>215</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
         <v>220</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="str">
         <f>Master!G3</f>
         <v>bjenks</v>
@@ -4182,7 +4182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="str">
         <f>Master!G4</f>
         <v>bswift</v>
@@ -4220,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="str">
         <f>Master!G5</f>
         <v>barmstrong</v>
@@ -4258,7 +4258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="str">
         <f>Master!G6</f>
         <v>fmason</v>
@@ -4296,7 +4296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="57" t="str">
         <f>Master!G7</f>
         <v>gjackson</v>
@@ -4334,7 +4334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="57" t="str">
         <f>Master!G8</f>
         <v>hbaldwin</v>
@@ -4372,7 +4372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="str">
         <f>Master!G9</f>
         <v>hrandall</v>
@@ -4410,7 +4410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="str">
         <f>Master!G10</f>
         <v>jwood</v>
@@ -4448,7 +4448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="str">
         <f>Master!G11</f>
         <v>jperiod</v>
@@ -4486,7 +4486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="str">
         <f>Master!G12</f>
         <v>jhaddon</v>
@@ -4524,7 +4524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="str">
         <f>Master!G13</f>
         <v>jmorse</v>
@@ -4562,7 +4562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="str">
         <f>Master!G14</f>
         <v>jsharp</v>
@@ -4600,7 +4600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="str">
         <f>Master!G15</f>
         <v>mbaggert</v>
@@ -4638,7 +4638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="57" t="str">
         <f>Master!G16</f>
         <v>mnestor</v>
@@ -4676,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="str">
         <f>Master!G17</f>
         <v>mblair</v>
@@ -4714,7 +4714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="str">
         <f>Master!G18</f>
         <v>mdelazes</v>
@@ -4752,7 +4752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="str">
         <f>Master!G19</f>
         <v>nnewton</v>
@@ -4790,7 +4790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="str">
         <f>Master!G20</f>
         <v>rsampson</v>
@@ -4828,7 +4828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="str">
         <f>Master!G21</f>
         <v>smalloy</v>
@@ -4866,7 +4866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="str">
         <f>Master!G22</f>
         <v>tswift</v>
@@ -4904,7 +4904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="57" t="str">
         <f>Master!G23</f>
         <v>wdamon</v>
@@ -4942,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="str">
         <f>Master!G24</f>
         <v>wcrawford</v>
@@ -4996,15 +4996,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.75" customWidth="1"/>
+    <col min="7" max="7" width="27.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>231</v>
       </c>
@@ -5053,7 +5053,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>231</v>
       </c>
@@ -5079,7 +5079,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>231</v>
       </c>
@@ -5105,7 +5105,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>231</v>
       </c>
@@ -5131,7 +5131,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>231</v>
       </c>
@@ -5157,7 +5157,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>231</v>
       </c>
@@ -5183,7 +5183,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>231</v>
       </c>
@@ -5209,7 +5209,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>231</v>
       </c>
@@ -5235,7 +5235,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>231</v>
       </c>
@@ -5261,7 +5261,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>231</v>
       </c>
@@ -5287,7 +5287,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>231</v>
       </c>
@@ -5313,7 +5313,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>231</v>
       </c>
@@ -5339,7 +5339,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>231</v>
       </c>
@@ -5365,7 +5365,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>231</v>
       </c>
@@ -5391,7 +5391,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>231</v>
       </c>
@@ -5417,7 +5417,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>231</v>
       </c>
@@ -5443,7 +5443,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>231</v>
       </c>
@@ -5469,7 +5469,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>231</v>
       </c>
@@ -5495,7 +5495,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>231</v>
       </c>
@@ -5521,7 +5521,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>231</v>
       </c>
@@ -5547,7 +5547,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>231</v>
       </c>
@@ -5573,7 +5573,7 @@
 Swift Construction Company</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>231</v>
       </c>

</xml_diff>